<commit_message>
The test row is removed.
</commit_message>
<xml_diff>
--- a/data/Reports.xlsx
+++ b/data/Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25385C9-0E40-4A38-AF0B-E38803660D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4040E60-FB46-4A21-AD30-E103931C8A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="258">
   <si>
     <t>Year</t>
   </si>
@@ -794,9 +794,6 @@
   </si>
   <si>
     <t>https://maps.app.goo.gl/TPjgki8dog5mWmFv5</t>
-  </si>
-  <si>
-    <t>jerhti</t>
   </si>
 </sst>
 </file>
@@ -1254,11 +1251,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2725,20 +2722,6 @@
         <v>257</v>
       </c>
       <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="17">
-        <v>2027</v>
-      </c>
-      <c r="B51" s="17">
-        <v>1</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>257</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>